<commit_message>
Fixed payment method with current date
Fixed payment method with current date
</commit_message>
<xml_diff>
--- a/test_data/make_payment.xlsx
+++ b/test_data/make_payment.xlsx
@@ -7,8 +7,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -423,14 +421,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20.77734375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="13.88671875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="17.5546875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="6" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="16" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="26.44140625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="15.88671875" bestFit="1" customWidth="1" min="6" max="6"/>
@@ -497,47 +495,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
WIP 8 & 9
</commit_message>
<xml_diff>
--- a/test_data/make_payment.xlsx
+++ b/test_data/make_payment.xlsx
@@ -475,17 +475,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>75c44810a32a3d6447df</t>
+          <t>7f065c23251bf386d439</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+74267426006</t>
+          <t>+74267426011</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Automation User 10</t>
+          <t>Automation User 11</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mobile test 1 to 7 and web base page fix
</commit_message>
<xml_diff>
--- a/test_data/make_payment.xlsx
+++ b/test_data/make_payment.xlsx
@@ -475,17 +475,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7f065c23251bf386d439</t>
+          <t>677f5c84fc34afaac4ae</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+74267426011</t>
+          <t>+74267426016</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Automation User 11</t>
+          <t>Automation User 16</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-05</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes for web tests
</commit_message>
<xml_diff>
--- a/test_data/make_payment.xlsx
+++ b/test_data/make_payment.xlsx
@@ -475,27 +475,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1b29e9245dbd466654c7</t>
+          <t>75c44810a32a3d6447df</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+74267426019</t>
+          <t>+74267426016</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Automation User 19</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+          <t>Automation User 10</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-02-16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to testdata and mobile capabilities
</commit_message>
<xml_diff>
--- a/test_data/make_payment.xlsx
+++ b/test_data/make_payment.xlsx
@@ -475,25 +475,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>75c44810a32a3d6447df</t>
+          <t>ece91ac614c097c9eaed</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+74267426016</t>
+          <t>+74267426018</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Automation User 10</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>100</v>
+          <t>Automation User 18</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
exception handled for opportunities
</commit_message>
<xml_diff>
--- a/test_data/make_payment.xlsx
+++ b/test_data/make_payment.xlsx
@@ -475,27 +475,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ece91ac614c097c9eaed</t>
+          <t>75c44810a32a3d6447df</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+74267426018</t>
+          <t>+74267426016</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Automation User 18</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+          <t>Automation User 10</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>

</xml_diff>